<commit_message>
new common features excel
</commit_message>
<xml_diff>
--- a/info/info.xlsx
+++ b/info/info.xlsx
@@ -735,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1103,10 +1103,10 @@
       <c r="B20" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="6" t="n">
@@ -1123,10 +1123,10 @@
       <c r="B21" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>85</v>
       </c>
       <c r="E21" s="6" t="n">
@@ -1150,13 +1150,13 @@
       <c r="B23" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="8" t="s">
         <v>90</v>
       </c>
       <c r="F23" s="9" t="s">
@@ -1170,13 +1170,13 @@
       <c r="B24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F24" s="9" t="s">
@@ -1190,10 +1190,10 @@
       <c r="B25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="8" t="s">
         <v>99</v>
       </c>
       <c r="E25" s="6" t="n">

</xml_diff>